<commit_message>
added basis sets graphs
</commit_message>
<xml_diff>
--- a/gas_phase_hcl_ccsd.xlsx
+++ b/gas_phase_hcl_ccsd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/github_thesis_graph/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/Thesis_graphs_binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6AE65E-5864-C344-B66B-FC6B1EA3C6DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF0F579-5466-7E47-BC56-0004BE3951CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="520" windowWidth="22440" windowHeight="14920" xr2:uid="{C1ADF71C-6822-4348-A305-5C9E8C2279D3}"/>
+    <workbookView xWindow="5480" yWindow="700" windowWidth="22440" windowHeight="14920" xr2:uid="{C1ADF71C-6822-4348-A305-5C9E8C2279D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,10 +45,10 @@
     <t>Gasphase_p_hcl_acv3z_dc</t>
   </si>
   <si>
-    <t>Gasphase_p_hcl_d_aug_acv3z_x2c</t>
+    <t>Gasphase_p_hcl_d_aug_acv3z_x2camf</t>
   </si>
   <si>
-    <t>Gasphase_p_hcl_d_aug_acv4z_x2c</t>
+    <t>Gasphase_p_hcl_d_aug_acv4z_x2camf</t>
   </si>
 </sst>
 </file>
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216E1151-E718-094E-AE0A-6B8FFA0D72FC}">
   <dimension ref="B4:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>